<commit_message>
Changes added to webservice.owl
</commit_message>
<xml_diff>
--- a/doc/All Inclusive.xlsx
+++ b/doc/All Inclusive.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="404" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="392" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -5040,9 +5040,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.5764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.878431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.6627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="1">
@@ -6098,16 +6098,16 @@
   </sheetPr>
   <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A87" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A87" xSplit="0" ySplit="-1"/>
-      <selection activeCell="G109" activeCellId="0" pane="topLeft" sqref="G109"/>
-      <selection activeCell="A87" activeCellId="0" pane="bottomLeft" sqref="A87"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A63" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A63" xSplit="0" ySplit="-1"/>
+      <selection activeCell="B70" activeCellId="0" pane="topLeft" sqref="B70"/>
+      <selection activeCell="A63" activeCellId="0" pane="bottomLeft" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="20" width="10.878431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="62.7607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="20" width="10.878431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="20" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="63.2823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="20" width="10.9725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8493,16 +8493,16 @@
   </sheetPr>
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A40" xSplit="0" ySplit="-1"/>
-      <selection activeCell="B54" activeCellId="0" pane="topLeft" sqref="B54"/>
-      <selection activeCell="A40" activeCellId="0" pane="bottomLeft" sqref="A40"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
+      <selection activeCell="D18" activeCellId="0" pane="topLeft" sqref="D18"/>
+      <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="60.5803921568627"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.6627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="61.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="20">
@@ -10907,14 +10907,14 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A13" xSplit="0" ySplit="-1"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A13" activeCellId="0" pane="bottomLeft" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="20">
@@ -11858,15 +11858,15 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="36" width="10.878431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="57.2392156862745"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="112" width="10.878431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="36" width="10.878431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="36" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="57.7098039215686"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="112" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="36" width="10.9725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="1">
@@ -12730,7 +12730,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="20" width="10.878431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="20" width="10.9725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Changed Curation Status added to Editor Notes as: Readi for OBI-ws v1.0
</commit_message>
<xml_diff>
--- a/doc/All Inclusive.xlsx
+++ b/doc/All Inclusive.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="282" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="190" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -288,7 +288,7 @@
     <t>Other/Super classes added</t>
   </si>
   <si>
-    <t>OBI-WS : v1.0 </t>
+    <t>OBI-WS : v1.0.0</t>
   </si>
   <si>
     <t>Lower Triangular Matrix</t>
@@ -329,6 +329,9 @@
     <t>N/a</t>
   </si>
   <si>
+    <t>OBI-WS : v1.0</t>
+  </si>
+  <si>
     <t>Scoring Matrix</t>
   </si>
   <si>
@@ -627,9 +630,6 @@
       </rPr>
       <t xml:space="preserve"> that describes the aim to study the equivalence between sites of molecular sequences including nucleic acid and protein sequence.</t>
     </r>
-  </si>
-  <si>
-    <t>OBI-WS : v1.0</t>
   </si>
   <si>
     <t>multiple sequence alignment objective</t>
@@ -4994,9 +4994,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.7058823529412"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.0156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.0627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.6" outlineLevel="0" r="1">
@@ -6052,16 +6052,16 @@
   </sheetPr>
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A94" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A94" xSplit="0" ySplit="-1"/>
-      <selection activeCell="D115" activeCellId="0" pane="topLeft" sqref="D115"/>
-      <selection activeCell="A94" activeCellId="0" pane="bottomLeft" sqref="A94"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="20" width="11.0156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="63.5490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="20" width="11.0156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="20" width="11.0627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="63.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="20" width="11.0627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -6223,10 +6223,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="12" s="36">
       <c r="A12" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>88</v>
@@ -6237,7 +6237,7 @@
         <v>87</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H12" s="35" t="s">
         <v>91</v>
@@ -6245,7 +6245,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="13" s="36">
       <c r="A13" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>89</v>
@@ -6256,10 +6256,10 @@
       <c r="D13" s="16"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H13" s="35" t="s">
         <v>91</v>
@@ -6267,10 +6267,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="14" s="36">
       <c r="A14" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>88</v>
@@ -6278,10 +6278,10 @@
       <c r="D14" s="16"/>
       <c r="E14" s="35"/>
       <c r="F14" s="35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H14" s="35" t="s">
         <v>91</v>
@@ -6289,10 +6289,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="15" s="36">
       <c r="A15" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>88</v>
@@ -6300,19 +6300,19 @@
       <c r="D15" s="16"/>
       <c r="E15" s="35"/>
       <c r="F15" s="35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H15" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="16" s="36">
       <c r="A16" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>88</v>
@@ -6320,10 +6320,10 @@
       <c r="D16" s="16"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H16" s="35" t="s">
         <v>91</v>
@@ -6331,10 +6331,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="17" s="36">
       <c r="A17" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>88</v>
@@ -6342,10 +6342,10 @@
       <c r="D17" s="16"/>
       <c r="E17" s="35"/>
       <c r="F17" s="35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H17" s="35" t="s">
         <v>91</v>
@@ -6353,10 +6353,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="18" s="36">
       <c r="A18" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C18" s="34" t="s">
         <v>88</v>
@@ -6364,10 +6364,10 @@
       <c r="D18" s="16"/>
       <c r="E18" s="35"/>
       <c r="F18" s="35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H18" s="35" t="s">
         <v>91</v>
@@ -6375,10 +6375,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="19" s="36">
       <c r="A19" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>88</v>
@@ -6386,10 +6386,10 @@
       <c r="D19" s="16"/>
       <c r="E19" s="35"/>
       <c r="F19" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H19" s="35" t="s">
         <v>91</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="20" s="36">
       <c r="A20" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>36</v>
@@ -6408,10 +6408,10 @@
       <c r="D20" s="16"/>
       <c r="E20" s="35"/>
       <c r="F20" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H20" s="35" t="s">
         <v>91</v>
@@ -6419,10 +6419,10 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="21" s="36">
       <c r="A21" s="38" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>88</v>
@@ -6430,10 +6430,10 @@
       <c r="D21" s="16"/>
       <c r="E21" s="35"/>
       <c r="F21" s="35" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H21" s="35" t="s">
         <v>91</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="22" s="36">
       <c r="A22" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>119</v>
@@ -6452,7 +6452,7 @@
       <c r="D22" s="16"/>
       <c r="E22" s="35"/>
       <c r="F22" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G22" s="35" t="s">
         <v>120</v>
@@ -6463,7 +6463,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="23" s="36">
       <c r="A23" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>121</v>
@@ -6474,7 +6474,7 @@
       <c r="D23" s="16"/>
       <c r="E23" s="35"/>
       <c r="F23" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G23" s="35" t="s">
         <v>122</v>
@@ -6485,7 +6485,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="24" s="36">
       <c r="A24" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>123</v>
@@ -6507,7 +6507,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="25" s="36">
       <c r="A25" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>46</v>
@@ -6529,7 +6529,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="26" s="36">
       <c r="A26" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>19</v>
@@ -6540,7 +6540,7 @@
       <c r="D26" s="35"/>
       <c r="E26" s="35"/>
       <c r="F26" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>126</v>
@@ -6551,7 +6551,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="27" s="36">
       <c r="A27" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>127</v>
@@ -6573,7 +6573,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="28" s="36">
       <c r="A28" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>130</v>
@@ -6595,7 +6595,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="29" s="36">
       <c r="A29" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>132</v>
@@ -6617,7 +6617,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="30" s="36">
       <c r="A30" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>135</v>
@@ -6639,7 +6639,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="31" s="36">
       <c r="A31" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>137</v>
@@ -6661,7 +6661,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="32" s="36">
       <c r="A32" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>139</v>
@@ -6683,7 +6683,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="33" s="36">
       <c r="A33" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>141</v>
@@ -6705,7 +6705,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="34" s="36">
       <c r="A34" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>143</v>
@@ -6727,7 +6727,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="35" s="36">
       <c r="A35" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>145</v>
@@ -6738,7 +6738,7 @@
       <c r="D35" s="35"/>
       <c r="E35" s="35"/>
       <c r="F35" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>146</v>
@@ -6749,7 +6749,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="36" s="36">
       <c r="A36" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>147</v>
@@ -6760,7 +6760,7 @@
       <c r="D36" s="35"/>
       <c r="E36" s="35"/>
       <c r="F36" s="35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>148</v>
@@ -6771,7 +6771,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="37" s="36">
       <c r="A37" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B37" s="41" t="s">
         <v>149</v>
@@ -6782,7 +6782,7 @@
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
       <c r="F37" s="35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G37" s="42" t="s">
         <v>150</v>
@@ -6839,7 +6839,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="42" s="36">
       <c r="A42" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>152</v>
@@ -6850,7 +6850,7 @@
       <c r="D42" s="16"/>
       <c r="E42" s="35"/>
       <c r="F42" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>154</v>
@@ -6873,7 +6873,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="44" s="36">
       <c r="A44" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>156</v>
@@ -6922,7 +6922,7 @@
         <v>161</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>162</v>
@@ -6933,7 +6933,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="47" s="36">
       <c r="A47" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>18</v>
@@ -6948,7 +6948,7 @@
         <v>164</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>165</v>
@@ -6984,7 +6984,7 @@
         <v>168</v>
       </c>
       <c r="F49" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G49" s="35" t="s">
         <v>169</v>
@@ -7019,7 +7019,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="51" s="36">
       <c r="A51" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>20</v>
@@ -7045,7 +7045,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="52" s="36">
       <c r="A52" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>21</v>
@@ -7109,7 +7109,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="55" s="36">
       <c r="A55" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>23</v>
@@ -7135,7 +7135,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="56" s="36">
       <c r="A56" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>24</v>
@@ -7161,7 +7161,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="57" s="36">
       <c r="A57" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>25</v>
@@ -7187,7 +7187,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="58" s="36">
       <c r="A58" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>26</v>
@@ -7213,7 +7213,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="59" s="36">
       <c r="A59" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>27</v>
@@ -7253,7 +7253,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="61" s="36">
       <c r="A61" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B61" s="16" t="s">
         <v>28</v>
@@ -7279,7 +7279,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="62" s="36">
       <c r="A62" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B62" s="16" t="s">
         <v>29</v>
@@ -7305,7 +7305,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="63" s="36">
       <c r="A63" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>30</v>
@@ -7331,7 +7331,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="64" s="36">
       <c r="A64" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B64" s="16" t="s">
         <v>31</v>
@@ -7371,7 +7371,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="66" s="36">
       <c r="A66" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>32</v>
@@ -7397,7 +7397,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="67" s="36">
       <c r="A67" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>33</v>
@@ -7423,7 +7423,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="68" s="36">
       <c r="A68" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>34</v>
@@ -7449,7 +7449,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="69" s="36">
       <c r="A69" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>35</v>
@@ -7488,7 +7488,7 @@
         <v>227</v>
       </c>
       <c r="F70" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>169</v>
@@ -7537,7 +7537,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="73" s="36">
       <c r="A73" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>37</v>
@@ -7562,7 +7562,6 @@
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="74" s="36">
-      <c r="A74" s="0"/>
       <c r="B74" s="16"/>
       <c r="C74" s="35"/>
       <c r="D74" s="16"/>
@@ -7601,7 +7600,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="77" s="36">
       <c r="A77" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B77" s="16" t="s">
         <v>237</v>
@@ -7612,7 +7611,7 @@
       <c r="D77" s="16"/>
       <c r="E77" s="35"/>
       <c r="F77" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G77" s="16" t="s">
         <v>239</v>
@@ -7637,7 +7636,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="79" s="36">
       <c r="A79" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B79" s="16" t="s">
         <v>38</v>
@@ -7648,7 +7647,7 @@
       <c r="D79" s="35"/>
       <c r="E79" s="35"/>
       <c r="F79" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G79" s="16" t="s">
         <v>240</v>
@@ -7709,7 +7708,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18" outlineLevel="0" r="83" s="36">
       <c r="A83" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B83" s="16" t="s">
         <v>39</v>
@@ -7773,7 +7772,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="17" outlineLevel="0" r="87" s="36">
       <c r="A87" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B87" s="16" t="s">
         <v>243</v>
@@ -7784,7 +7783,7 @@
       <c r="D87" s="16"/>
       <c r="E87" s="35"/>
       <c r="F87" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G87" s="16" t="s">
         <v>245</v>
@@ -7807,7 +7806,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="89" s="36">
       <c r="A89" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B89" s="16" t="s">
         <v>40</v>
@@ -7818,7 +7817,7 @@
       <c r="D89" s="35"/>
       <c r="E89" s="35"/>
       <c r="F89" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G89" s="16" t="s">
         <v>246</v>
@@ -7881,7 +7880,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="93" s="36">
       <c r="A93" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B93" s="16" t="s">
         <v>41</v>
@@ -7907,7 +7906,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="94" s="36">
       <c r="A94" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B94" s="16" t="s">
         <v>42</v>
@@ -7931,7 +7930,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="95" s="36">
       <c r="A95" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B95" s="16" t="s">
         <v>43</v>
@@ -7995,7 +7994,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="98" s="36">
       <c r="A98" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B98" s="16" t="s">
         <v>44</v>
@@ -8057,7 +8056,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="17" outlineLevel="0" r="102" s="36">
       <c r="A102" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B102" s="16" t="s">
         <v>264</v>
@@ -8100,7 +8099,7 @@
       <c r="D104" s="35"/>
       <c r="E104" s="35"/>
       <c r="F104" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G104" s="16" t="s">
         <v>169</v>
@@ -8179,7 +8178,7 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="109" s="36">
       <c r="A109" s="38" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B109" s="16" t="s">
         <v>45</v>
@@ -8509,9 +8508,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.7058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="61.3333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="61.5843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="20">
@@ -8658,7 +8657,7 @@
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>291</v>
@@ -8869,7 +8868,7 @@
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G23" s="16" t="s">
         <v>311</v>
@@ -8939,7 +8938,7 @@
         <v>161</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>314</v>
@@ -8964,7 +8963,7 @@
         <v>316</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>314</v>
@@ -10891,12 +10890,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="20">
       <c r="A1" s="79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>454</v>
@@ -11029,7 +11028,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="35"/>
       <c r="F11" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>460</v>
@@ -11840,15 +11839,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="36" width="11.0156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="57.9490196078431"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="117" width="11.0156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="36" width="11.0156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="36" width="11.0627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="36" width="58.1843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="117" width="11.0627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="36" width="11.0627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="1">
       <c r="A1" s="117" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>470</v>
@@ -11970,7 +11969,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="35"/>
       <c r="F11" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>480</v>
@@ -12004,7 +12003,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>483</v>
@@ -12064,7 +12063,7 @@
         <v>490</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G16" s="35" t="s">
         <v>491</v>
@@ -12272,7 +12271,7 @@
       <c r="D29" s="35"/>
       <c r="E29" s="35"/>
       <c r="F29" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>514</v>
@@ -12304,7 +12303,7 @@
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
       <c r="F31" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>517</v>
@@ -12707,7 +12706,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="20" width="11.0156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="20" width="11.0627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="1">
@@ -12837,7 +12836,7 @@
       <c r="D9" s="19"/>
       <c r="E9" s="35"/>
       <c r="F9" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>546</v>
@@ -13239,7 +13238,7 @@
       <c r="D36" s="19"/>
       <c r="E36" s="35"/>
       <c r="F36" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G36" s="19" t="s">
         <v>574</v>
@@ -13269,7 +13268,7 @@
       <c r="D38" s="19"/>
       <c r="E38" s="35"/>
       <c r="F38" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>577</v>
@@ -13389,7 +13388,7 @@
       <c r="D47" s="19"/>
       <c r="E47" s="35"/>
       <c r="F47" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G47" s="19" t="s">
         <v>582</v>
@@ -13419,7 +13418,7 @@
       <c r="D49" s="19"/>
       <c r="E49" s="35"/>
       <c r="F49" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G49" s="19" t="s">
         <v>585</v>
@@ -13559,7 +13558,7 @@
       <c r="D59" s="19"/>
       <c r="E59" s="35"/>
       <c r="F59" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G59" s="19" t="s">
         <v>588</v>
@@ -13587,7 +13586,7 @@
       <c r="D61" s="19"/>
       <c r="E61" s="35"/>
       <c r="F61" s="35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G61" s="19" t="s">
         <v>590</v>
@@ -13703,7 +13702,7 @@
       <c r="D70" s="19"/>
       <c r="E70" s="35"/>
       <c r="F70" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G70" s="19" t="s">
         <v>596</v>
@@ -13837,7 +13836,7 @@
       <c r="D81" s="19"/>
       <c r="E81" s="35"/>
       <c r="F81" s="35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G81" s="18" t="s">
         <v>600</v>

</xml_diff>

<commit_message>
Terms added for phylip Protdist, protpars, consense and neighbor, Ontology reasoned for consistency
</commit_message>
<xml_diff>
--- a/doc/All Inclusive.xlsx
+++ b/doc/All Inclusive.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="962" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="16" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="951" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -4485,7 +4485,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> that aims to compute a protein distance matrix for a multiple sequence alignemnt using a sutable amino acid replacement model.</t>
+      <t xml:space="preserve"> that aims to compute a protein distance matrix for a multiple sequence alignemnt using a suitable amino acid replacement model.</t>
     </r>
   </si>
   <si>
@@ -4496,9 +4496,6 @@
   </si>
   <si>
     <t>model</t>
-  </si>
-  <si>
-    <t>plan specification</t>
   </si>
   <si>
     <r>
@@ -4513,7 +4510,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">plan specification</t>
+      <t xml:space="preserve">symbol</t>
     </r>
     <r>
       <rPr>
@@ -4523,7 +4520,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> that is an empirical model for protein evolution in which amino acids mutate according to some predefined probabilities that depend on the amino acid itself.</t>
+      <t xml:space="preserve"> that specifies an empirical model for protein evolution in which amino acids mutate according to some predefined probabilities that depend on the amino acid itself.</t>
     </r>
   </si>
   <si>
@@ -4570,7 +4567,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> that stores the evolutionary distance between each pair of protein sequences, with each species starting on a new line with the species name, followed by the distances to the species in order.</t>
+      <t xml:space="preserve"> that stores the evolutionary distance between each pair of protein sequences, with each species starting on a new line with the species name, followed by the distance to the species in order.</t>
     </r>
   </si>
   <si>
@@ -4610,7 +4607,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">web service execution</t>
+      <t xml:space="preserve">run phylip execution</t>
     </r>
     <r>
       <rPr>
@@ -4645,7 +4642,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">sequence analysis data transformation</t>
+      <t xml:space="preserve">sequence analysis objective</t>
     </r>
     <r>
       <rPr>
@@ -4717,7 +4714,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> which is a tree that represents evolutionary relationships between species, where usually the length of branches of the tree signify evolutionary distance.</t>
+      <t xml:space="preserve"> which is a tree that represents evolutionary relationships between species, where the length of branches of the tree can signify evolutionary distance.</t>
     </r>
   </si>
   <si>
@@ -4757,7 +4754,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">plan specification</t>
+      <t xml:space="preserve">data set</t>
     </r>
     <r>
       <rPr>
@@ -4793,7 +4790,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">A </t>
+      <t xml:space="preserve">A</t>
     </r>
     <r>
       <rPr>
@@ -4804,7 +4801,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">web service execution</t>
+      <t xml:space="preserve"> run phylip execution </t>
     </r>
     <r>
       <rPr>
@@ -4814,11 +4811,11 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> that constructs a consensus tree that summarizes the  agreement between two or more phylogenetic trees.</t>
-    </r>
-  </si>
-  <si>
-    <t>consensus tree construction methods</t>
+      <t xml:space="preserve">that constructs a consensus tree that summarizes the  agreement between two or more phylogenetic trees.</t>
+    </r>
+  </si>
+  <si>
+    <t>consensus tree construction algorithm</t>
   </si>
   <si>
     <t>consensusType</t>
@@ -4856,6 +4853,9 @@
     <t>consenseRootedTrees</t>
   </si>
   <si>
+    <t>consensus tree construction methods</t>
+  </si>
+  <si>
     <t>retrieveConsenseResult</t>
   </si>
   <si>
@@ -4869,7 +4869,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Consensus trees are </t>
+      <t xml:space="preserve">Consensus tree is a</t>
     </r>
     <r>
       <rPr>
@@ -4880,7 +4880,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">phylogenetic tree</t>
+      <t xml:space="preserve"> phylogenetic tree </t>
     </r>
     <r>
       <rPr>
@@ -4890,7 +4890,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">s that summarize agremment between two or more trees.</t>
+      <t xml:space="preserve">that summarize agremment between two or more phylogenetic trees.</t>
     </r>
   </si>
 </sst>
@@ -6083,7 +6083,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -6268,11 +6268,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76770038"/>
-        <c:axId val="72695186"/>
+        <c:axId val="46094903"/>
+        <c:axId val="30322542"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76770038"/>
+        <c:axId val="46094903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6280,7 +6280,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72695186"/>
+        <c:crossAx val="30322542"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -6294,7 +6294,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72695186"/>
+        <c:axId val="30322542"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6311,7 +6311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76770038"/>
+        <c:crossAx val="46094903"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -6348,15 +6348,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1219320</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:colOff>1273320</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>179280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>387360</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:colOff>440640</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>214920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6364,8 +6364,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1219320" y="4069440"/>
-        <a:ext cx="5789160" cy="2458440"/>
+        <a:off x="1273320" y="2725560"/>
+        <a:ext cx="5801040" cy="1477080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6390,9 +6390,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9529411764706"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="8.96470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="9.03529411764706"/>
+    <col collapsed="false" hidden="false" max="16" min="11" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -6997,15 +6999,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.5803921568627"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="12.2039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="20.7294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="14.7058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="14.556862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="67.7921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="9.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.7098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="12.3058823529412"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="20.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="14.8274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="13.6470588235294"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="14.678431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="68.3529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="9.50196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8141,15 +8143,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8881,15 +8883,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -9267,16 +9269,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -9988,20 +9990,20 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="H45" activeCellId="0" pane="topLeft" sqref="H45"/>
+      <selection activeCell="H16" activeCellId="0" pane="topLeft" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -10094,14 +10096,14 @@
       <c r="H6" s="153"/>
       <c r="I6" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="7">
       <c r="A7" s="9" t="s">
         <v>662</v>
       </c>
       <c r="B7" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="154" t="s">
         <v>663</v>
       </c>
       <c r="D7" s="102"/>
@@ -10150,14 +10152,14 @@
       <c r="H10" s="40"/>
       <c r="I10" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="A11" s="9" t="s">
         <v>666</v>
       </c>
       <c r="B11" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="51" t="s">
         <v>667</v>
       </c>
       <c r="D11" s="40" t="s">
@@ -10186,10 +10188,10 @@
       <c r="H12" s="2"/>
       <c r="I12" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="9"/>
       <c r="B13" s="170"/>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="51" t="s">
         <v>670</v>
       </c>
       <c r="E13" s="98"/>
@@ -10236,14 +10238,14 @@
       </c>
       <c r="I15" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="A16" s="9" t="s">
         <v>672</v>
       </c>
       <c r="B16" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="154" t="s">
         <v>673</v>
       </c>
       <c r="D16" s="40" t="s">
@@ -10256,13 +10258,13 @@
         <v>148</v>
       </c>
       <c r="G16" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>675</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="I16" s="64" t="s">
         <v>676</v>
-      </c>
-      <c r="I16" s="64" t="s">
-        <v>677</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="17">
@@ -10272,7 +10274,7 @@
         <v>491</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E17" s="98"/>
       <c r="F17" s="40"/>
@@ -10287,7 +10289,7 @@
         <v>491</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E18" s="98"/>
       <c r="F18" s="40"/>
@@ -10387,7 +10389,7 @@
         <v>667</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E26" s="98"/>
       <c r="F26" s="40"/>
@@ -10564,7 +10566,7 @@
         <v>127</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E39" s="98"/>
       <c r="F39" s="40"/>
@@ -10616,7 +10618,7 @@
         <v>236</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="40"/>
@@ -10637,7 +10639,7 @@
       <c r="H44" s="171"/>
       <c r="I44" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="45">
       <c r="A45" s="9" t="s">
         <v>666</v>
       </c>
@@ -10645,10 +10647,10 @@
         <v>53</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E45" s="40"/>
       <c r="F45" s="40"/>
@@ -10656,7 +10658,7 @@
         <v>56</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I45" s="153"/>
     </row>
@@ -10700,7 +10702,7 @@
         <v>136</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E49" s="40"/>
       <c r="F49" s="39"/>
@@ -10763,7 +10765,7 @@
       <c r="B54" s="99"/>
       <c r="C54" s="154"/>
       <c r="D54" s="40" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E54" s="40"/>
       <c r="F54" s="40"/>
@@ -10789,7 +10791,7 @@
       <c r="B56" s="99"/>
       <c r="C56" s="154"/>
       <c r="D56" s="40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40"/>
@@ -10847,21 +10849,21 @@
   </sheetPr>
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="H11" activeCellId="0" pane="topLeft" sqref="H11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A28" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="C48" activeCellId="0" pane="topLeft" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -10869,7 +10871,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>660</v>
@@ -10885,7 +10887,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -11000,24 +11002,24 @@
       <c r="H10" s="40"/>
       <c r="I10" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="A11" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="51" t="s">
         <v>690</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="40" t="s">
         <v>691</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>692</v>
       </c>
       <c r="E11" s="98"/>
       <c r="F11" s="40"/>
       <c r="G11" s="40" t="s">
-        <v>73</v>
+        <v>663</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I11" s="40"/>
     </row>
@@ -11034,21 +11036,21 @@
       <c r="H12" s="2"/>
       <c r="I12" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="B13" s="170"/>
+      <c r="C13" s="51" t="s">
         <v>694</v>
-      </c>
-      <c r="B13" s="170"/>
-      <c r="C13" s="12" t="s">
-        <v>695</v>
       </c>
       <c r="E13" s="98"/>
       <c r="F13" s="40"/>
       <c r="G13" s="40" t="s">
+        <v>695</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>696</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>697</v>
       </c>
       <c r="I13" s="40"/>
     </row>
@@ -11069,10 +11071,10 @@
       <c r="A15" s="9"/>
       <c r="B15" s="99"/>
       <c r="C15" s="154" t="s">
+        <v>697</v>
+      </c>
+      <c r="D15" s="40" t="s">
         <v>698</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>699</v>
       </c>
       <c r="E15" s="98" t="s">
         <v>147</v>
@@ -11082,7 +11084,7 @@
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="64" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I15" s="153"/>
     </row>
@@ -11093,7 +11095,7 @@
         <v>232</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E16" s="98" t="s">
         <v>147</v>
@@ -11103,7 +11105,7 @@
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="179" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I16" s="64"/>
     </row>
@@ -11114,7 +11116,7 @@
         <v>491</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E17" s="98" t="s">
         <v>221</v>
@@ -11133,7 +11135,7 @@
         <v>491</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E18" s="98" t="s">
         <v>221</v>
@@ -11152,7 +11154,7 @@
         <v>491</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E19" s="40" t="s">
         <v>221</v>
@@ -11254,7 +11256,7 @@
       <c r="B27" s="170"/>
       <c r="C27" s="51"/>
       <c r="D27" s="40" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E27" s="98"/>
       <c r="F27" s="40"/>
@@ -11303,10 +11305,10 @@
       <c r="A31" s="9"/>
       <c r="B31" s="99"/>
       <c r="C31" s="154" t="s">
+        <v>697</v>
+      </c>
+      <c r="D31" s="40" t="s">
         <v>698</v>
-      </c>
-      <c r="D31" s="40" t="s">
-        <v>699</v>
       </c>
       <c r="E31" s="98" t="s">
         <v>147</v>
@@ -11316,7 +11318,7 @@
       </c>
       <c r="G31" s="40"/>
       <c r="H31" s="64" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I31" s="153"/>
     </row>
@@ -11327,7 +11329,7 @@
         <v>232</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E32" s="98" t="s">
         <v>147</v>
@@ -11337,7 +11339,7 @@
       </c>
       <c r="G32" s="40"/>
       <c r="H32" s="179" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I32" s="64"/>
     </row>
@@ -11433,7 +11435,7 @@
         <v>127</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E40" s="98"/>
       <c r="F40" s="40"/>
@@ -11485,7 +11487,7 @@
         <v>236</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="40"/>
@@ -11506,14 +11508,14 @@
       <c r="H45" s="171"/>
       <c r="I45" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="46">
       <c r="A46" s="9"/>
       <c r="B46" s="99"/>
-      <c r="C46" s="40" t="s">
+      <c r="C46" s="154" t="s">
+        <v>707</v>
+      </c>
+      <c r="D46" s="40" t="s">
         <v>708</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>709</v>
       </c>
       <c r="E46" s="40"/>
       <c r="F46" s="40"/>
@@ -11521,7 +11523,7 @@
         <v>122</v>
       </c>
       <c r="H46" s="171" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="I46" s="153" t="s">
         <v>55</v>
@@ -11532,7 +11534,7 @@
       <c r="B47" s="42"/>
       <c r="C47" s="40"/>
       <c r="D47" s="40" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E47" s="40"/>
       <c r="F47" s="40"/>
@@ -11580,7 +11582,7 @@
         <v>136</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E51" s="40"/>
       <c r="F51" s="39"/>
@@ -11643,7 +11645,7 @@
       <c r="B56" s="99"/>
       <c r="C56" s="154"/>
       <c r="D56" s="40" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40"/>
@@ -11669,7 +11671,7 @@
       <c r="B58" s="99"/>
       <c r="C58" s="154"/>
       <c r="D58" s="40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
@@ -11726,21 +11728,21 @@
   </sheetPr>
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="C31" activeCellId="0" pane="topLeft" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -11748,7 +11750,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>660</v>
@@ -11764,7 +11766,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -11884,7 +11886,7 @@
       <c r="B11" s="42"/>
       <c r="C11" s="12"/>
       <c r="D11" s="40" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E11" s="98"/>
       <c r="F11" s="40"/>
@@ -11908,8 +11910,8 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="9"/>
       <c r="B13" s="170"/>
-      <c r="C13" s="12" t="s">
-        <v>695</v>
+      <c r="C13" s="51" t="s">
+        <v>694</v>
       </c>
       <c r="E13" s="98"/>
       <c r="F13" s="40"/>
@@ -11937,7 +11939,7 @@
         <v>284</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E15" s="98" t="s">
         <v>147</v>
@@ -11951,16 +11953,16 @@
       </c>
       <c r="I15" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
       <c r="A16" s="19" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="154" t="s">
+        <v>716</v>
+      </c>
+      <c r="D16" s="40" t="s">
         <v>717</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>718</v>
       </c>
       <c r="E16" s="98" t="s">
         <v>147</v>
@@ -11969,10 +11971,10 @@
         <v>198</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>675</v>
+        <v>122</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I16" s="64"/>
     </row>
@@ -11983,7 +11985,7 @@
         <v>321</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E17" s="98"/>
       <c r="F17" s="40" t="s">
@@ -12085,7 +12087,7 @@
         <v>127</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E25" s="98"/>
       <c r="F25" s="40"/>
@@ -12137,7 +12139,7 @@
         <v>236</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
@@ -12162,16 +12164,16 @@
       <c r="A31" s="9"/>
       <c r="B31" s="99"/>
       <c r="C31" s="154" t="s">
+        <v>707</v>
+      </c>
+      <c r="D31" s="40" t="s">
         <v>708</v>
-      </c>
-      <c r="D31" s="40" t="s">
-        <v>709</v>
       </c>
       <c r="E31" s="40"/>
       <c r="F31" s="40"/>
       <c r="G31" s="40"/>
       <c r="H31" s="171" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I31" s="153"/>
     </row>
@@ -12180,7 +12182,7 @@
       <c r="B32" s="42"/>
       <c r="C32" s="40"/>
       <c r="D32" s="40" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
@@ -12228,7 +12230,7 @@
         <v>136</v>
       </c>
       <c r="D36" s="75" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E36" s="40"/>
       <c r="F36" s="39"/>
@@ -12291,7 +12293,7 @@
       <c r="B41" s="99"/>
       <c r="C41" s="154"/>
       <c r="D41" s="40" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
@@ -12317,7 +12319,7 @@
       <c r="B43" s="99"/>
       <c r="C43" s="154"/>
       <c r="D43" s="40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="40"/>
@@ -12373,21 +12375,21 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="H9" activeCellId="0" pane="topLeft" sqref="H9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="D18" activeCellId="0" pane="topLeft" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.6862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="15.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.9725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.3098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="48.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -12395,7 +12397,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>660</v>
@@ -12411,7 +12413,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -12493,22 +12495,22 @@
       <c r="H7" s="40"/>
       <c r="I7" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
       <c r="A8" s="9"/>
       <c r="B8" s="42"/>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="51" t="s">
+        <v>724</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>725</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>726</v>
       </c>
       <c r="E8" s="98"/>
       <c r="F8" s="40"/>
       <c r="G8" s="40" t="s">
-        <v>73</v>
+        <v>663</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I8" s="40"/>
     </row>
@@ -12528,8 +12530,8 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="9"/>
       <c r="B10" s="170"/>
-      <c r="C10" s="12" t="s">
-        <v>695</v>
+      <c r="C10" s="51" t="s">
+        <v>694</v>
       </c>
       <c r="E10" s="98"/>
       <c r="F10" s="40"/>
@@ -12553,8 +12555,8 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
       <c r="A12" s="9"/>
       <c r="B12" s="99"/>
-      <c r="C12" s="40" t="s">
-        <v>708</v>
+      <c r="C12" s="154" t="s">
+        <v>707</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>595</v>
@@ -12569,14 +12571,14 @@
       <c r="H12" s="64"/>
       <c r="I12" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="9"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="154" t="s">
+        <v>727</v>
+      </c>
+      <c r="D13" s="40" t="s">
         <v>728</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>729</v>
       </c>
       <c r="E13" s="40" t="s">
         <v>147</v>
@@ -12585,10 +12587,10 @@
         <v>148</v>
       </c>
       <c r="G13" s="40" t="s">
+        <v>729</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>730</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>731</v>
       </c>
       <c r="I13" s="64"/>
     </row>
@@ -12682,7 +12684,7 @@
       <c r="B21" s="170"/>
       <c r="C21" s="51"/>
       <c r="D21" s="40" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E21" s="98"/>
       <c r="F21" s="40"/>
@@ -12706,8 +12708,8 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="23">
       <c r="A23" s="9"/>
       <c r="B23" s="170"/>
-      <c r="C23" s="12" t="s">
-        <v>695</v>
+      <c r="C23" s="51" t="s">
+        <v>694</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="98"/>
@@ -12732,8 +12734,8 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="25">
       <c r="A25" s="9"/>
       <c r="B25" s="99"/>
-      <c r="C25" s="40" t="s">
-        <v>708</v>
+      <c r="C25" s="154" t="s">
+        <v>707</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>595</v>
@@ -12751,11 +12753,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="26">
       <c r="A26" s="9"/>
       <c r="B26" s="42"/>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="154" t="s">
+        <v>732</v>
+      </c>
+      <c r="D26" s="40" t="s">
         <v>728</v>
-      </c>
-      <c r="D26" s="40" t="s">
-        <v>729</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>147</v>
@@ -12911,7 +12913,7 @@
         <v>236</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
@@ -12932,10 +12934,10 @@
       <c r="H39" s="171"/>
       <c r="I39" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="40">
       <c r="A40" s="9"/>
       <c r="B40" s="99"/>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="154" t="s">
         <v>734</v>
       </c>
       <c r="D40" s="40" t="s">
@@ -13003,7 +13005,7 @@
         <v>136</v>
       </c>
       <c r="D45" s="75" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E45" s="40"/>
       <c r="F45" s="39"/>
@@ -13066,7 +13068,7 @@
       <c r="B50" s="99"/>
       <c r="C50" s="154"/>
       <c r="D50" s="40" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
@@ -13092,7 +13094,7 @@
       <c r="B52" s="99"/>
       <c r="C52" s="154"/>
       <c r="D52" s="40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E52" s="40"/>
       <c r="F52" s="40"/>
@@ -13152,15 +13154,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.4901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="67.3490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="14.843137254902"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="19" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.7647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="67.9098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="14.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="1">
@@ -15832,12 +15834,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="18.5372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="22.0588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.243137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="22.243137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -16505,14 +16507,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.5372549019608"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="58.3921568627451"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="13.9686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.243137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="58.878431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -17265,14 +17267,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.5372549019608"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="58.3921568627451"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="13.9686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.243137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.6941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="58.878431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -18154,14 +18156,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="22.0588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="53.5294117647059"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="22.243137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="53.9764705882353"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -19967,16 +19969,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7372549019608"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4039215686275"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="47.6352941176471"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="18.0862745098039"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="48.0313725490196"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -21282,13 +21284,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.756862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="13.9686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="18.6745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="61.4745098039216"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.6078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.9019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="18.8313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="61.9764705882353"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -22484,18 +22486,18 @@
   </sheetPr>
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
       <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.756862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="13.9686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="18.6745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.6156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="61.4745098039216"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.6078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.9019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="18.8313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="61.9764705882353"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.7176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
one new term added. phylip execuion identifier
</commit_message>
<xml_diff>
--- a/doc/All Inclusive.xlsx
+++ b/doc/All Inclusive.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="16" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="951" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="732" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="742">
   <si>
     <t>MSA</t>
   </si>
@@ -4510,7 +4510,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">symbol</t>
+      <t xml:space="preserve">matrix</t>
     </r>
     <r>
       <rPr>
@@ -4520,7 +4520,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> that specifies an empirical model for protein evolution in which amino acids mutate according to some predefined probabilities that depend on the amino acid itself.</t>
+      <t xml:space="preserve"> that represents an empirical model for protein evolution in which amino acids mutate according to some predefined probabilities.</t>
     </r>
   </si>
   <si>
@@ -4531,6 +4531,35 @@
   </si>
   <si>
     <t>CoeffOfVariation</t>
+  </si>
+  <si>
+    <t>phylip execution identifier</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="true"/>
+        <color rgb="00000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">web service execution identifier </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="00000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">that uniquely identifies a submitted a phylip web service execution.</t>
+    </r>
   </si>
   <si>
     <t>protdistDefaultParameters</t>
@@ -4718,6 +4747,9 @@
     </r>
   </si>
   <si>
+    <t>http://en.wikipedia.org/wiki/Newick_format</t>
+  </si>
+  <si>
     <t>outfile</t>
   </si>
   <si>
@@ -4811,7 +4843,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">that constructs a consensus tree that summarizes the  agreement between two or more phylogenetic trees.</t>
+      <t xml:space="preserve">that constructs a consensus tree that summarizes the  agreement of the branching order between two or more phylogenetic trees.</t>
     </r>
   </si>
   <si>
@@ -4850,6 +4882,9 @@
     </r>
   </si>
   <si>
+    <t>Clatogram</t>
+  </si>
+  <si>
     <t>consenseRootedTrees</t>
   </si>
   <si>
@@ -4869,7 +4904,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Consensus tree is a</t>
+      <t xml:space="preserve">A </t>
     </r>
     <r>
       <rPr>
@@ -4880,7 +4915,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve"> phylogenetic tree </t>
+      <t xml:space="preserve">phylogenetic tree t</t>
     </r>
     <r>
       <rPr>
@@ -4890,7 +4925,7 @@
         <color rgb="00000000"/>
         <sz val="11"/>
       </rPr>
-      <t xml:space="preserve">that summarize agremment between two or more phylogenetic trees.</t>
+      <t xml:space="preserve">hat is a clatogram which summarize agremment between two or more phylogenetic trees.</t>
     </r>
   </si>
 </sst>
@@ -4901,7 +4936,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="73">
+  <fonts count="74">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -5435,6 +5470,13 @@
       <sz val="10"/>
       <u val="single"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -5509,7 +5551,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -6010,6 +6052,9 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="73" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -6083,7 +6128,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -6268,11 +6313,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="46094903"/>
-        <c:axId val="30322542"/>
+        <c:axId val="2157854"/>
+        <c:axId val="77214615"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46094903"/>
+        <c:axId val="2157854"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6280,7 +6325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30322542"/>
+        <c:crossAx val="77214615"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -6294,7 +6339,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30322542"/>
+        <c:axId val="77214615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6311,7 +6356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46094903"/>
+        <c:crossAx val="2157854"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -6348,15 +6393,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1273320</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>179280</xdr:rowOff>
+      <xdr:colOff>1354320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>440640</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>214920</xdr:rowOff>
+      <xdr:colOff>520560</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>194760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6364,8 +6409,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1273320" y="2725560"/>
-        <a:ext cx="5801040" cy="1477080"/>
+        <a:off x="1354320" y="1659960"/>
+        <a:ext cx="5879880" cy="651600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6385,16 +6430,16 @@
   </sheetPr>
   <dimension ref="A2:U20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="P7" activeCellId="0" pane="topLeft" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="9.03529411764706"/>
-    <col collapsed="false" hidden="false" max="16" min="11" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="9.14117647058824"/>
+    <col collapsed="false" hidden="false" max="16" min="11" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -6600,7 +6645,7 @@
         <v>2</v>
       </c>
       <c r="P5" s="12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="2" t="n">
         <v>3</v>
@@ -6662,7 +6707,7 @@
         <v>2</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="2" t="n">
         <v>3</v>
@@ -6678,7 +6723,7 @@
       </c>
       <c r="U6" s="0" t="n">
         <f aca="false">SUM(B6:T6)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="7">
@@ -6999,15 +7044,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.7098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="12.3058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="20.9019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="14.8274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="13.6470588235294"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="14.678431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="68.3529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="9.50196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.9058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="21.1607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="15.0156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="13.8117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="18.156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="69.2078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="9.62352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8143,15 +8188,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8883,15 +8928,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -9269,16 +9314,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -9989,21 +10034,21 @@
   </sheetPr>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="H16" activeCellId="0" pane="topLeft" sqref="H16"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A37" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="C43" activeCellId="0" pane="topLeft" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -10096,7 +10141,7 @@
       <c r="H6" s="153"/>
       <c r="I6" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="7">
       <c r="A7" s="9" t="s">
         <v>662</v>
       </c>
@@ -10152,7 +10197,7 @@
       <c r="H10" s="40"/>
       <c r="I10" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
       <c r="A11" s="9" t="s">
         <v>666</v>
       </c>
@@ -10188,7 +10233,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
       <c r="A13" s="9"/>
       <c r="B13" s="170"/>
       <c r="C13" s="51" t="s">
@@ -10258,7 +10303,7 @@
         <v>148</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>675</v>
@@ -10325,15 +10370,19 @@
       <c r="A21" s="9"/>
       <c r="B21" s="99"/>
       <c r="C21" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D21" s="40" t="s">
         <v>282</v>
       </c>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="2"/>
+      <c r="G21" s="179" t="s">
+        <v>236</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>680</v>
+      </c>
       <c r="I21" s="153"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="22">
@@ -10389,7 +10438,7 @@
         <v>667</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="E26" s="98"/>
       <c r="F26" s="40"/>
@@ -10505,7 +10554,9 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="34">
       <c r="A34" s="9"/>
       <c r="B34" s="99"/>
-      <c r="C34" s="154"/>
+      <c r="C34" s="154" t="s">
+        <v>679</v>
+      </c>
       <c r="D34" s="40"/>
       <c r="E34" s="40"/>
       <c r="F34" s="40"/>
@@ -10566,7 +10617,7 @@
         <v>127</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E39" s="98"/>
       <c r="F39" s="40"/>
@@ -10615,10 +10666,10 @@
       <c r="A43" s="9"/>
       <c r="B43" s="99"/>
       <c r="C43" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="40"/>
@@ -10639,7 +10690,7 @@
       <c r="H44" s="171"/>
       <c r="I44" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="45">
       <c r="A45" s="9" t="s">
         <v>666</v>
       </c>
@@ -10647,10 +10698,10 @@
         <v>53</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="E45" s="40"/>
       <c r="F45" s="40"/>
@@ -10658,7 +10709,7 @@
         <v>56</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="I45" s="153"/>
     </row>
@@ -10702,7 +10753,7 @@
         <v>136</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E49" s="40"/>
       <c r="F49" s="39"/>
@@ -10765,7 +10816,7 @@
       <c r="B54" s="99"/>
       <c r="C54" s="154"/>
       <c r="D54" s="40" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E54" s="40"/>
       <c r="F54" s="40"/>
@@ -10791,7 +10842,7 @@
       <c r="B56" s="99"/>
       <c r="C56" s="154"/>
       <c r="D56" s="40" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40"/>
@@ -10849,21 +10900,21 @@
   </sheetPr>
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A28" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="C48" activeCellId="0" pane="topLeft" sqref="C48"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="C44" activeCellId="0" pane="topLeft" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -10871,7 +10922,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>660</v>
@@ -10887,7 +10938,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -11002,16 +11053,16 @@
       <c r="H10" s="40"/>
       <c r="I10" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
       <c r="A11" s="9" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="51" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E11" s="98"/>
       <c r="F11" s="40"/>
@@ -11019,7 +11070,7 @@
         <v>663</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="I11" s="40"/>
     </row>
@@ -11036,21 +11087,21 @@
       <c r="H12" s="2"/>
       <c r="I12" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
       <c r="A13" s="9" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B13" s="170"/>
       <c r="C13" s="51" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E13" s="98"/>
       <c r="F13" s="40"/>
       <c r="G13" s="40" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="I13" s="40"/>
     </row>
@@ -11071,10 +11122,10 @@
       <c r="A15" s="9"/>
       <c r="B15" s="99"/>
       <c r="C15" s="154" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E15" s="98" t="s">
         <v>147</v>
@@ -11084,7 +11135,7 @@
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="64" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="I15" s="153"/>
     </row>
@@ -11095,7 +11146,7 @@
         <v>232</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E16" s="98" t="s">
         <v>147</v>
@@ -11104,8 +11155,8 @@
         <v>148</v>
       </c>
       <c r="G16" s="40"/>
-      <c r="H16" s="179" t="s">
-        <v>701</v>
+      <c r="H16" s="180" t="s">
+        <v>703</v>
       </c>
       <c r="I16" s="64"/>
     </row>
@@ -11116,7 +11167,7 @@
         <v>491</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="E17" s="98" t="s">
         <v>221</v>
@@ -11135,7 +11186,7 @@
         <v>491</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="E18" s="98" t="s">
         <v>221</v>
@@ -11154,7 +11205,7 @@
         <v>491</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="E19" s="40" t="s">
         <v>221</v>
@@ -11194,7 +11245,7 @@
       <c r="A22" s="9"/>
       <c r="B22" s="99"/>
       <c r="C22" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>282</v>
@@ -11256,7 +11307,7 @@
       <c r="B27" s="170"/>
       <c r="C27" s="51"/>
       <c r="D27" s="40" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="E27" s="98"/>
       <c r="F27" s="40"/>
@@ -11305,10 +11356,10 @@
       <c r="A31" s="9"/>
       <c r="B31" s="99"/>
       <c r="C31" s="154" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E31" s="98" t="s">
         <v>147</v>
@@ -11318,7 +11369,7 @@
       </c>
       <c r="G31" s="40"/>
       <c r="H31" s="64" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="I31" s="153"/>
     </row>
@@ -11329,7 +11380,7 @@
         <v>232</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E32" s="98" t="s">
         <v>147</v>
@@ -11338,8 +11389,8 @@
         <v>198</v>
       </c>
       <c r="G32" s="40"/>
-      <c r="H32" s="179" t="s">
-        <v>701</v>
+      <c r="H32" s="180" t="s">
+        <v>703</v>
       </c>
       <c r="I32" s="64"/>
     </row>
@@ -11371,7 +11422,7 @@
       <c r="A35" s="9"/>
       <c r="B35" s="99"/>
       <c r="C35" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D35" s="40" t="s">
         <v>282</v>
@@ -11435,7 +11486,7 @@
         <v>127</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="E40" s="98"/>
       <c r="F40" s="40"/>
@@ -11484,10 +11535,10 @@
       <c r="A44" s="9"/>
       <c r="B44" s="99"/>
       <c r="C44" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="40"/>
@@ -11508,14 +11559,14 @@
       <c r="H45" s="171"/>
       <c r="I45" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="46">
       <c r="A46" s="9"/>
       <c r="B46" s="99"/>
       <c r="C46" s="154" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E46" s="40"/>
       <c r="F46" s="40"/>
@@ -11523,10 +11574,10 @@
         <v>122</v>
       </c>
       <c r="H46" s="171" t="s">
-        <v>709</v>
-      </c>
-      <c r="I46" s="153" t="s">
-        <v>55</v>
+        <v>711</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>712</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="47">
@@ -11534,7 +11585,7 @@
       <c r="B47" s="42"/>
       <c r="C47" s="40"/>
       <c r="D47" s="40" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="E47" s="40"/>
       <c r="F47" s="40"/>
@@ -11582,7 +11633,7 @@
         <v>136</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E51" s="40"/>
       <c r="F51" s="39"/>
@@ -11645,7 +11696,7 @@
       <c r="B56" s="99"/>
       <c r="C56" s="154"/>
       <c r="D56" s="40" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="40"/>
@@ -11671,7 +11722,7 @@
       <c r="B58" s="99"/>
       <c r="C58" s="154"/>
       <c r="D58" s="40" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
@@ -11710,6 +11761,7 @@
     <hyperlink display="http://mango.ctegd.uga.edu/jkissingLab/SWS/services.html#phylip" location="phylip" ref="D1" r:id="rId1"/>
     <hyperlink display="http://evolution.genetics.washington.edu/phylip/doc/neighbor.html" ref="A11" r:id="rId2"/>
     <hyperlink display="http://en.wikipedia.org/wiki/Phylogenetic_tree#Unrooted_tree" location="Unrooted_tree" ref="A13" r:id="rId3"/>
+    <hyperlink display="http://en.wikipedia.org/wiki/Newick_format" ref="I46" r:id="rId4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -11729,20 +11781,20 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="C31" activeCellId="0" pane="topLeft" sqref="C31"/>
+      <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -11750,7 +11802,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>660</v>
@@ -11766,7 +11818,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -11886,7 +11938,7 @@
       <c r="B11" s="42"/>
       <c r="C11" s="12"/>
       <c r="D11" s="40" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="E11" s="98"/>
       <c r="F11" s="40"/>
@@ -11911,7 +11963,7 @@
       <c r="A13" s="9"/>
       <c r="B13" s="170"/>
       <c r="C13" s="51" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E13" s="98"/>
       <c r="F13" s="40"/>
@@ -11939,7 +11991,7 @@
         <v>284</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="E15" s="98" t="s">
         <v>147</v>
@@ -11953,16 +12005,16 @@
       </c>
       <c r="I15" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
       <c r="A16" s="19" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="154" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="E16" s="98" t="s">
         <v>147</v>
@@ -11974,7 +12026,7 @@
         <v>122</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="I16" s="64"/>
     </row>
@@ -11985,7 +12037,7 @@
         <v>321</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="E17" s="98"/>
       <c r="F17" s="40" t="s">
@@ -12023,7 +12075,7 @@
       <c r="A20" s="9"/>
       <c r="B20" s="99"/>
       <c r="C20" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D20" s="40" t="s">
         <v>282</v>
@@ -12087,7 +12139,7 @@
         <v>127</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="E25" s="98"/>
       <c r="F25" s="40"/>
@@ -12136,10 +12188,10 @@
       <c r="A29" s="9"/>
       <c r="B29" s="99"/>
       <c r="C29" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
@@ -12164,16 +12216,16 @@
       <c r="A31" s="9"/>
       <c r="B31" s="99"/>
       <c r="C31" s="154" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="E31" s="40"/>
       <c r="F31" s="40"/>
       <c r="G31" s="40"/>
       <c r="H31" s="171" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="I31" s="153"/>
     </row>
@@ -12182,7 +12234,7 @@
       <c r="B32" s="42"/>
       <c r="C32" s="40"/>
       <c r="D32" s="40" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40"/>
@@ -12230,7 +12282,7 @@
         <v>136</v>
       </c>
       <c r="D36" s="75" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E36" s="40"/>
       <c r="F36" s="39"/>
@@ -12293,7 +12345,7 @@
       <c r="B41" s="99"/>
       <c r="C41" s="154"/>
       <c r="D41" s="40" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E41" s="40"/>
       <c r="F41" s="40"/>
@@ -12319,7 +12371,7 @@
       <c r="B43" s="99"/>
       <c r="C43" s="154"/>
       <c r="D43" s="40" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="40"/>
@@ -12375,21 +12427,21 @@
   </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="D18" activeCellId="0" pane="topLeft" sqref="D18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="G16" activeCellId="0" pane="topLeft" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="20.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.4156862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.156862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -12397,7 +12449,7 @@
         <v>77</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>660</v>
@@ -12413,7 +12465,7 @@
         <v>38</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -12495,14 +12547,14 @@
       <c r="H7" s="40"/>
       <c r="I7" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
       <c r="A8" s="9"/>
       <c r="B8" s="42"/>
       <c r="C8" s="51" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="E8" s="98"/>
       <c r="F8" s="40"/>
@@ -12510,7 +12562,7 @@
         <v>663</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="I8" s="40"/>
     </row>
@@ -12531,7 +12583,7 @@
       <c r="A10" s="9"/>
       <c r="B10" s="170"/>
       <c r="C10" s="51" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E10" s="98"/>
       <c r="F10" s="40"/>
@@ -12556,7 +12608,7 @@
       <c r="A12" s="9"/>
       <c r="B12" s="99"/>
       <c r="C12" s="154" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>595</v>
@@ -12571,14 +12623,14 @@
       <c r="H12" s="64"/>
       <c r="I12" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
       <c r="A13" s="9"/>
       <c r="B13" s="42"/>
       <c r="C13" s="154" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="E13" s="40" t="s">
         <v>147</v>
@@ -12587,12 +12639,14 @@
         <v>148</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>730</v>
-      </c>
-      <c r="I13" s="64"/>
+        <v>733</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="A14" s="9"/>
@@ -12622,14 +12676,14 @@
       <c r="A16" s="9"/>
       <c r="B16" s="99"/>
       <c r="C16" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D16" s="40" t="s">
         <v>282</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="G16" s="179"/>
       <c r="H16" s="2"/>
       <c r="I16" s="153"/>
     </row>
@@ -12684,7 +12738,7 @@
       <c r="B21" s="170"/>
       <c r="C21" s="51"/>
       <c r="D21" s="40" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="E21" s="98"/>
       <c r="F21" s="40"/>
@@ -12709,7 +12763,7 @@
       <c r="A23" s="9"/>
       <c r="B23" s="170"/>
       <c r="C23" s="51" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="98"/>
@@ -12735,7 +12789,7 @@
       <c r="A25" s="9"/>
       <c r="B25" s="99"/>
       <c r="C25" s="154" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>595</v>
@@ -12754,10 +12808,10 @@
       <c r="A26" s="9"/>
       <c r="B26" s="42"/>
       <c r="C26" s="154" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="E26" s="40" t="s">
         <v>147</v>
@@ -12766,7 +12820,7 @@
         <v>148</v>
       </c>
       <c r="G26" s="40"/>
-      <c r="H26" s="179"/>
+      <c r="H26" s="180"/>
       <c r="I26" s="64"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="27">
@@ -12797,7 +12851,7 @@
       <c r="A29" s="9"/>
       <c r="B29" s="99"/>
       <c r="C29" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D29" s="40" t="s">
         <v>282</v>
@@ -12861,7 +12915,7 @@
         <v>127</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
       <c r="E34" s="98"/>
       <c r="F34" s="40"/>
@@ -12910,10 +12964,10 @@
       <c r="A38" s="9"/>
       <c r="B38" s="99"/>
       <c r="C38" s="154" t="s">
-        <v>236</v>
+        <v>679</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
@@ -12938,17 +12992,17 @@
       <c r="A40" s="9"/>
       <c r="B40" s="99"/>
       <c r="C40" s="154" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="E40" s="40"/>
       <c r="G40" s="40" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="I40" s="153" t="s">
         <v>55</v>
@@ -13005,7 +13059,7 @@
         <v>136</v>
       </c>
       <c r="D45" s="75" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="E45" s="40"/>
       <c r="F45" s="39"/>
@@ -13068,7 +13122,7 @@
       <c r="B50" s="99"/>
       <c r="C50" s="154"/>
       <c r="D50" s="40" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
@@ -13094,7 +13148,7 @@
       <c r="B52" s="99"/>
       <c r="C52" s="154"/>
       <c r="D52" s="40" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E52" s="40"/>
       <c r="F52" s="40"/>
@@ -13154,15 +13208,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.7647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="67.9098039215686"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="14.9647058823529"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="19" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="33.1725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="68.7529411764706"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="15.1450980392157"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="1">
@@ -15834,12 +15888,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.243137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="22.243137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="22.5254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -16507,14 +16561,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.243137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="58.878431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0078431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="59.6117647058824"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.2549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -17267,14 +17321,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.243137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.6941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="58.878431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0078431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="59.6117647058824"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.2549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -18156,14 +18210,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="22.243137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="53.9764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="22.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7137254901961"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="54.6509803921569"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -19969,16 +20023,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="18.0862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8392156862745"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7058823529412"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8196078431373"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="48.0313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="18.3058823529412"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8352941176471"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6627450980392"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="48.6313725490196"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -21284,13 +21338,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.9019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="18.8313725490196"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="61.9764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.7529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="17.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.2549019607843"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="19.0666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="62.7529411764706"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -22491,13 +22545,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.9019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="18.8313725490196"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.7176470588235"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="61.9764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.7529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="17.1176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.2549019607843"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="19.0666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="62.7529411764706"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
terms for phylip curated
</commit_message>
<xml_diff>
--- a/doc/All Inclusive.xlsx
+++ b/doc/All Inclusive.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="732" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="962" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -4936,7 +4936,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="74">
+  <fonts count="71">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -5034,17 +5034,6 @@
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="14"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="18"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -5470,13 +5459,6 @@
       <sz val="10"/>
       <u val="single"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -5590,9 +5572,9 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5602,11 +5584,11 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -5615,31 +5597,31 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="20" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="22" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="19" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="21" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5647,7 +5629,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5657,11 +5639,24 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="16" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="14" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="22" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="25" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5669,38 +5664,25 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="25" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="25" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="18" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="28" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="9" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="22" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="27" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="28" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="27" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="27" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="27" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="20" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="25" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="30" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5715,15 +5697,15 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="17" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="32" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="30" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="33" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="31" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5731,20 +5713,20 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="35" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="33" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="12" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="36" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="34" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="17" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5755,29 +5737,29 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="16" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="14" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="9" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="16" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="14" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="19" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="24" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="22" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5785,33 +5767,33 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="19" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="38" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="36" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="39" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="37" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="40" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="38" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="40" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="3" fontId="38" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="42" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="40" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -5821,20 +5803,20 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="43" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="41" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="22" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="44" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="20" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="45" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="21" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="42" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="18" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="43" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5844,20 +5826,20 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="19" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="19" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5873,30 +5855,30 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="46" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="44" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="44" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="42" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="45" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="45" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="46" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="44" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="46" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="44" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="35" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="33" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -5909,13 +5891,37 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="46" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="48" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="49" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="49" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="50" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="35" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="51" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="52" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="55" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="56" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5923,41 +5929,17 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="37" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="59" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="30" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="53" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="54" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="57" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="58" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="54" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="61" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="32" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="35" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="4" fontId="33" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="10" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="62" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="60" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5966,16 +5948,16 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="61" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="62" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="63" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="64" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="65" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="47" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="45" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5984,58 +5966,58 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="26" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="24" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="25" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="25" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="23" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="67" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="65" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="35" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="33" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="35" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="33" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="26" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="24" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="36" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="34" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="57" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="55" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="68" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="66" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="26" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="24" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="35" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="69" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="33" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="67" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="19" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="11" numFmtId="164" xfId="0">
@@ -6044,15 +6026,15 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="71" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="72" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="69" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="70" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="73" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="68" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
@@ -6114,8 +6096,8 @@
       <rgbColor rgb="00FF9900"/>
       <rgbColor rgb="00E46C0A"/>
       <rgbColor rgb="00666666"/>
-      <rgbColor rgb="00B3B3B3"/>
-      <rgbColor rgb="00004586"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
       <rgbColor rgb="00339966"/>
       <rgbColor rgb="00003300"/>
       <rgbColor rgb="00333300"/>
@@ -6128,301 +6110,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1"/>
-              <a:t>Total New Terms Proposed</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Summary!$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total New Terms Proposed</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Summary!$B$19:$T$19</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>clustalW</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>muscle</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>tcoffee</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clustalO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>WuBlast</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>NCBIBlast</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>PsiBlast</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>FASTA</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>signalP</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>InterProscan</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>phobious</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>WSDBFetch</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Filtersequences</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>WSConverters</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>ProtDist</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Neighbor</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Consense</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Protpars</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>ClustalW2Phylogeny</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Summary!$B$20:$T$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="2157854"/>
-        <c:axId val="77214615"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2157854"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77214615"/>
-        <c:crossesAt val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="77214615"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2157854"/>
-        <c:crossesAt val="0"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-      </c:valAx>
-      <c:spPr>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:spPr/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1354320</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>520560</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>194760</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="1354320" y="1659960"/>
-        <a:ext cx="5879880" cy="651600"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -6430,16 +6117,16 @@
   </sheetPr>
   <dimension ref="A2:U20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="G1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
-      <selection activeCell="P7" activeCellId="0" pane="topLeft" sqref="P7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100">
+      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5607843137255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="9.14117647058824"/>
-    <col collapsed="false" hidden="false" max="16" min="11" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="16" min="11" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2">
@@ -7028,7 +6715,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7044,15 +6730,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.9058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="12.4549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="21.1607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="15.0156862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="13.8117647058824"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="14.8705882352941"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="18.156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="69.2078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="9.62352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.0352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="12.556862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="21.3333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="15.1372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="14.9960784313725"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="20" width="18.3058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="69.7803921568628"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="20" width="9.70980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8188,15 +7874,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -8928,15 +8614,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -9314,16 +9000,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -10039,16 +9725,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -10283,7 +9969,7 @@
       </c>
       <c r="I15" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
       <c r="A16" s="9" t="s">
         <v>672</v>
       </c>
@@ -10366,7 +10052,7 @@
       <c r="H20" s="171"/>
       <c r="I20" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="21">
       <c r="A21" s="9"/>
       <c r="B21" s="99"/>
       <c r="C21" s="154" t="s">
@@ -10905,16 +10591,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -11785,16 +11471,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -12432,16 +12118,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.1176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.321568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.2392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="13.9254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="49.7725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="13.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="13.3529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="19" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="19" width="14.0392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="50.1882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="19" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -12988,7 +12674,7 @@
       <c r="H39" s="171"/>
       <c r="I39" s="153"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="40">
       <c r="A40" s="9"/>
       <c r="B40" s="99"/>
       <c r="C40" s="154" t="s">
@@ -13208,15 +12894,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="33.1725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="68.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="15.1450980392157"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="19" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="33.4509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="69.3294117647059"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="15.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="19" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="1">
@@ -15888,12 +15574,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="22.5254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="19.0901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="22.7098039215686"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -16561,14 +16247,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5254901960784"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="59.6117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.2549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="19.0901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="60.0980392156863"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.3686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -17321,14 +17007,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5254901960784"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="59.6117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.2549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="19.0901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="60.0980392156863"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="112" width="14.3686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -18210,14 +17896,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="22.5254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7137254901961"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="54.6509803921569"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="22.7098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="55.1098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -20023,16 +19709,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="18.3058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8352941176471"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6627450980392"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="48.6313725490196"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="18.4588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.7647058823529"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="122" width="49.0352941176471"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="19">
@@ -21338,13 +21024,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="17.1176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.2549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="19.0666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="62.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.9647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="17.2588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.3686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="19.2235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="63.2745098039216"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="17.1019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">
@@ -22545,13 +22231,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="17.1176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.2549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="19.0666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.8588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="62.7529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="16.9647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="17.2588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="14.3686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="19.2235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="20" width="11.9607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="63.2745098039216"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="17.1019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="20" width="11.9607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1">

</xml_diff>